<commit_message>
add special attribute displayed, enabled, selected.
</commit_message>
<xml_diff>
--- a/asset/Google検索.xlsx
+++ b/asset/Google検索.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$E$6</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$E$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$E$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">Sheet1!$A$1:$E$7</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t xml:space="preserve">name[q]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">assert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ボタン[Google 検索]表示</t>
+  </si>
+  <si>
+    <t xml:space="preserve">is[true]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name[btnK#displayed]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ボタン[Google 検索]活性</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name[btnK#enabled]</t>
   </si>
   <si>
     <t xml:space="preserve">click</t>
@@ -109,9 +127,6 @@
     <t xml:space="preserve">name[btnK]</t>
   </si>
   <si>
-    <t xml:space="preserve">assert</t>
-  </si>
-  <si>
     <t xml:space="preserve">タイトル</t>
   </si>
   <si>
@@ -258,13 +273,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.65234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.03"/>
@@ -334,8 +349,11 @@
       <c r="C4" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="0" t="s">
+        <v>15</v>
+      </c>
       <c r="F4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -343,27 +361,58 @@
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>18</v>
-      </c>
-      <c r="F5" s="0" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="F6" s="4" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fullscreen capture, element capture
</commit_message>
<xml_diff>
--- a/asset/Google検索.xlsx
+++ b/asset/Google検索.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">capture</t>
   </si>
   <si>
-    <t xml:space="preserve"> ウインドウ</t>
+    <t xml:space="preserve">ウインドウ</t>
   </si>
   <si>
     <t xml:space="preserve">input</t>
@@ -447,7 +447,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>